<commit_message>
english planes focus icons
</commit_message>
<xml_diff>
--- a/BiceExpanded EXTRAS/BICE Tech List.xlsx
+++ b/BiceExpanded EXTRAS/BICE Tech List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chimera\Documents\Paradox Interactive\Hearts of Iron IV\mod\BlackICE-Expanded\BiceExpanded EXTRAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E534F9C9-8300-4247-80E6-1A24ABDC68DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3472DC-66E2-488C-8501-50EB389F863F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{120BDE58-771D-4E2C-9FD2-0BCD9B5D8EC1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22296" windowHeight="13176" xr2:uid="{120BDE58-771D-4E2C-9FD2-0BCD9B5D8EC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Industry" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="112">
   <si>
     <t>Tech Name</t>
   </si>
@@ -300,16 +300,91 @@
   </si>
   <si>
     <t>sub_industry3</t>
+  </si>
+  <si>
+    <t>wood_engines</t>
+  </si>
+  <si>
+    <t>wood_engines2</t>
+  </si>
+  <si>
+    <t>char_engines</t>
+  </si>
+  <si>
+    <t>fuel_silos</t>
+  </si>
+  <si>
+    <t>FLAG 300</t>
+  </si>
+  <si>
+    <t>FLAG 10</t>
+  </si>
+  <si>
+    <t>fuel_cans</t>
+  </si>
+  <si>
+    <t>fuel_silos2</t>
+  </si>
+  <si>
+    <t>fuel_silos3</t>
+  </si>
+  <si>
+    <t>fuel_silos4</t>
+  </si>
+  <si>
+    <t>fuel_silos5</t>
+  </si>
+  <si>
+    <t>fuel_refining</t>
+  </si>
+  <si>
+    <t>fuel_refining2</t>
+  </si>
+  <si>
+    <t>fuel_refining3</t>
+  </si>
+  <si>
+    <t>fuel_refining4</t>
+  </si>
+  <si>
+    <t>fuel_refining5</t>
+  </si>
+  <si>
+    <t>catalytic_cracking</t>
+  </si>
+  <si>
+    <t>commercial_catalytic_cracking</t>
+  </si>
+  <si>
+    <t>fluid_catalytic_cracking</t>
+  </si>
+  <si>
+    <t>construction1</t>
+  </si>
+  <si>
+    <t>defence_works</t>
+  </si>
+  <si>
+    <t>aa_emplacement_construction</t>
+  </si>
+  <si>
+    <t>ADD 40</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -374,20 +449,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{042549B0-C838-440F-910F-E3E035F893B0}" name="Table1" displayName="Table1" ref="A1:K75" totalsRowShown="0">
-  <autoFilter ref="A1:K75" xr:uid="{C89E43BA-120F-4DC0-A6DA-5AF10A372DE6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{042549B0-C838-440F-910F-E3E035F893B0}" name="Table1" displayName="Table1" ref="A1:K95" totalsRowShown="0">
+  <autoFilter ref="A1:K95" xr:uid="{C89E43BA-120F-4DC0-A6DA-5AF10A372DE6}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{BBD0135A-950C-45DB-9EA8-B23A1432BFFE}" name="Tech Name"/>
     <tableColumn id="2" xr3:uid="{52943816-45DD-4FF3-A8C5-C4736910B0F3}" name="Folder"/>
     <tableColumn id="3" xr3:uid="{ED58554E-F065-4A71-9C70-D140F04B9A92}" name="Year"/>
     <tableColumn id="4" xr3:uid="{C42EDC2F-B10A-4E06-9BAD-D1BED39BF075}" name="Cost"/>
     <tableColumn id="5" xr3:uid="{EF34E1DB-526B-4321-8E8F-8ED6B1249A52}" name="Base Prio"/>
-    <tableColumn id="11" xr3:uid="{A9BE7041-1DA8-4CF6-AD2E-9F1AC88CB0BC}" name="Prio -Y" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{83836DF1-0FD8-42BF-95BF-5D3393BBA7C1}" name="Prio 0 Y" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{C68A9217-D82C-45F2-A251-97E2E2917B20}" name="Prio 1 Y" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{F4EF635C-ED33-432F-8C8E-6A5920099464}" name="Prio 2 Y" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{A9BE7041-1DA8-4CF6-AD2E-9F1AC88CB0BC}" name="Prio -Y" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{83836DF1-0FD8-42BF-95BF-5D3393BBA7C1}" name="Prio 0 Y" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{C68A9217-D82C-45F2-A251-97E2E2917B20}" name="Prio 1 Y" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{F4EF635C-ED33-432F-8C8E-6A5920099464}" name="Prio 2 Y" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{316272FF-89BD-4226-A0EA-7EC288C6978B}" name="Total Prio"/>
-    <tableColumn id="10" xr3:uid="{432739BE-3B67-46D6-97BE-16B6F8A629E7}" name="% Change" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{432739BE-3B67-46D6-97BE-16B6F8A629E7}" name="% Change" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -690,26 +765,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C3C70DF-FE6D-4113-A583-B190C327E009}">
-  <dimension ref="A1:K75"/>
+  <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="1" customWidth="1"/>
-    <col min="7" max="9" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="1" customWidth="1"/>
+    <col min="7" max="9" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" customWidth="1"/>
+    <col min="11" max="11" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -744,7 +819,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -762,7 +837,7 @@
       </c>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -783,7 +858,7 @@
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -810,7 +885,7 @@
       </c>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -834,7 +909,7 @@
       </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -855,7 +930,7 @@
       </c>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -882,10 +957,13 @@
       </c>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
       <c r="C8">
         <v>40</v>
       </c>
@@ -900,10 +978,13 @@
       </c>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
       <c r="C9">
         <v>37</v>
       </c>
@@ -918,10 +999,13 @@
       </c>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
       <c r="C10">
         <v>42</v>
       </c>
@@ -936,10 +1020,13 @@
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
       <c r="C11">
         <v>37</v>
       </c>
@@ -960,10 +1047,13 @@
       </c>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
       <c r="C12">
         <v>41</v>
       </c>
@@ -978,10 +1068,13 @@
       </c>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
       <c r="C13">
         <v>42</v>
       </c>
@@ -996,10 +1089,13 @@
       </c>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>19</v>
       </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
       <c r="C14">
         <v>45</v>
       </c>
@@ -1014,10 +1110,13 @@
       </c>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
       <c r="C15">
         <v>38</v>
       </c>
@@ -1032,10 +1131,13 @@
       </c>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>21</v>
       </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
       <c r="C16">
         <v>39</v>
       </c>
@@ -1047,10 +1149,13 @@
       </c>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>22</v>
       </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
       <c r="C17">
         <v>36</v>
       </c>
@@ -1065,10 +1170,13 @@
       </c>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>23</v>
       </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
       <c r="C18">
         <v>37</v>
       </c>
@@ -1086,10 +1194,13 @@
       </c>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>28</v>
       </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
       <c r="C19">
         <v>39</v>
       </c>
@@ -1107,10 +1218,13 @@
       </c>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>29</v>
       </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
       <c r="C20">
         <v>41</v>
       </c>
@@ -1128,10 +1242,13 @@
       </c>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>31</v>
       </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
       <c r="C21">
         <v>43</v>
       </c>
@@ -1149,10 +1266,13 @@
       </c>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>32</v>
       </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
       <c r="C22">
         <v>43</v>
       </c>
@@ -1164,10 +1284,13 @@
       </c>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>33</v>
       </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
       <c r="C23">
         <v>44</v>
       </c>
@@ -1185,10 +1308,13 @@
       </c>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>34</v>
       </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
       <c r="C24">
         <v>45</v>
       </c>
@@ -1203,10 +1329,13 @@
       </c>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>35</v>
       </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
       <c r="C25">
         <v>37</v>
       </c>
@@ -1224,10 +1353,13 @@
       </c>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>36</v>
       </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
       <c r="C26">
         <v>37</v>
       </c>
@@ -1239,10 +1371,13 @@
       </c>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>37</v>
       </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
       <c r="C27">
         <v>39</v>
       </c>
@@ -1254,10 +1389,13 @@
       </c>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>38</v>
       </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
       <c r="C28">
         <v>38</v>
       </c>
@@ -1275,10 +1413,13 @@
       </c>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>39</v>
       </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
       <c r="C29">
         <v>39</v>
       </c>
@@ -1296,10 +1437,13 @@
       </c>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>40</v>
       </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
       <c r="C30">
         <v>41</v>
       </c>
@@ -1317,10 +1461,13 @@
       </c>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>41</v>
       </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
       <c r="C31">
         <v>41</v>
       </c>
@@ -1338,10 +1485,13 @@
       </c>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>42</v>
       </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
       <c r="C32">
         <v>43</v>
       </c>
@@ -1356,10 +1506,13 @@
       </c>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>43</v>
       </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
       <c r="C33">
         <v>36</v>
       </c>
@@ -1377,10 +1530,13 @@
       </c>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>44</v>
       </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
       <c r="C34">
         <v>37</v>
       </c>
@@ -1398,10 +1554,13 @@
       </c>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>47</v>
       </c>
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
       <c r="C35">
         <v>39</v>
       </c>
@@ -1419,10 +1578,13 @@
       </c>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>49</v>
       </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
       <c r="C36">
         <v>41</v>
       </c>
@@ -1440,10 +1602,13 @@
       </c>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>50</v>
       </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
       <c r="C37">
         <v>43</v>
       </c>
@@ -1461,10 +1626,13 @@
       </c>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>51</v>
       </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
       <c r="C38">
         <v>36</v>
       </c>
@@ -1482,10 +1650,13 @@
       </c>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>52</v>
       </c>
+      <c r="B39" t="s">
+        <v>6</v>
+      </c>
       <c r="C39">
         <v>37</v>
       </c>
@@ -1503,10 +1674,13 @@
       </c>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>53</v>
       </c>
+      <c r="B40" t="s">
+        <v>6</v>
+      </c>
       <c r="C40">
         <v>39</v>
       </c>
@@ -1524,10 +1698,13 @@
       </c>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>54</v>
       </c>
+      <c r="B41" t="s">
+        <v>6</v>
+      </c>
       <c r="C41">
         <v>41</v>
       </c>
@@ -1545,10 +1722,13 @@
       </c>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>55</v>
       </c>
+      <c r="B42" t="s">
+        <v>6</v>
+      </c>
       <c r="C42">
         <v>43</v>
       </c>
@@ -1566,10 +1746,13 @@
       </c>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>56</v>
       </c>
+      <c r="B43" t="s">
+        <v>6</v>
+      </c>
       <c r="C43">
         <v>36</v>
       </c>
@@ -1581,10 +1764,13 @@
       </c>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>57</v>
       </c>
+      <c r="B44" t="s">
+        <v>6</v>
+      </c>
       <c r="C44">
         <v>40</v>
       </c>
@@ -1599,10 +1785,13 @@
       </c>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>58</v>
       </c>
+      <c r="B45" t="s">
+        <v>6</v>
+      </c>
       <c r="C45">
         <v>44</v>
       </c>
@@ -1617,10 +1806,13 @@
       </c>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>59</v>
       </c>
+      <c r="B46" t="s">
+        <v>6</v>
+      </c>
       <c r="D46">
         <v>0.5</v>
       </c>
@@ -1629,10 +1821,13 @@
       </c>
       <c r="K46" s="1"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>60</v>
       </c>
+      <c r="B47" t="s">
+        <v>6</v>
+      </c>
       <c r="D47">
         <v>0.5</v>
       </c>
@@ -1641,10 +1836,13 @@
       </c>
       <c r="K47" s="1"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>61</v>
       </c>
+      <c r="B48" t="s">
+        <v>6</v>
+      </c>
       <c r="D48">
         <v>0.5</v>
       </c>
@@ -1653,10 +1851,13 @@
       </c>
       <c r="K48" s="1"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>62</v>
       </c>
+      <c r="B49" t="s">
+        <v>6</v>
+      </c>
       <c r="D49">
         <v>0.5</v>
       </c>
@@ -1665,10 +1866,13 @@
       </c>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>63</v>
       </c>
+      <c r="B50" t="s">
+        <v>6</v>
+      </c>
       <c r="D50">
         <v>0.5</v>
       </c>
@@ -1677,10 +1881,13 @@
       </c>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>64</v>
       </c>
+      <c r="B51" t="s">
+        <v>6</v>
+      </c>
       <c r="D51">
         <v>0.5</v>
       </c>
@@ -1689,10 +1896,13 @@
       </c>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>65</v>
       </c>
+      <c r="B52" t="s">
+        <v>6</v>
+      </c>
       <c r="D52">
         <v>0.5</v>
       </c>
@@ -1701,10 +1911,13 @@
       </c>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>66</v>
       </c>
+      <c r="B53" t="s">
+        <v>6</v>
+      </c>
       <c r="D53">
         <v>0.5</v>
       </c>
@@ -1713,10 +1926,13 @@
       </c>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>67</v>
       </c>
+      <c r="B54" t="s">
+        <v>6</v>
+      </c>
       <c r="D54">
         <v>0.5</v>
       </c>
@@ -1725,10 +1941,13 @@
       </c>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>68</v>
       </c>
+      <c r="B55" t="s">
+        <v>6</v>
+      </c>
       <c r="D55">
         <v>0.5</v>
       </c>
@@ -1737,10 +1956,13 @@
       </c>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>69</v>
       </c>
+      <c r="B56" t="s">
+        <v>6</v>
+      </c>
       <c r="D56">
         <v>0.5</v>
       </c>
@@ -1749,10 +1971,13 @@
       </c>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>70</v>
       </c>
+      <c r="B57" t="s">
+        <v>6</v>
+      </c>
       <c r="D57">
         <v>0.5</v>
       </c>
@@ -1761,10 +1986,13 @@
       </c>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>71</v>
       </c>
+      <c r="B58" t="s">
+        <v>6</v>
+      </c>
       <c r="D58">
         <v>0.5</v>
       </c>
@@ -1773,10 +2001,13 @@
       </c>
       <c r="K58" s="1"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>72</v>
       </c>
+      <c r="B59" t="s">
+        <v>6</v>
+      </c>
       <c r="D59">
         <v>0.5</v>
       </c>
@@ -1785,10 +2016,13 @@
       </c>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>73</v>
       </c>
+      <c r="B60" t="s">
+        <v>6</v>
+      </c>
       <c r="D60">
         <v>0.5</v>
       </c>
@@ -1797,10 +2031,13 @@
       </c>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>74</v>
       </c>
+      <c r="B61" t="s">
+        <v>6</v>
+      </c>
       <c r="D61">
         <v>0.5</v>
       </c>
@@ -1809,10 +2046,13 @@
       </c>
       <c r="K61" s="1"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>75</v>
       </c>
+      <c r="B62" t="s">
+        <v>6</v>
+      </c>
       <c r="D62">
         <v>0.5</v>
       </c>
@@ -1821,10 +2061,13 @@
       </c>
       <c r="K62" s="1"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>76</v>
       </c>
+      <c r="B63" t="s">
+        <v>6</v>
+      </c>
       <c r="D63">
         <v>0.5</v>
       </c>
@@ -1833,10 +2076,13 @@
       </c>
       <c r="K63" s="1"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>77</v>
       </c>
+      <c r="B64" t="s">
+        <v>6</v>
+      </c>
       <c r="D64">
         <v>0.5</v>
       </c>
@@ -1845,10 +2091,13 @@
       </c>
       <c r="K64" s="1"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>78</v>
       </c>
+      <c r="B65" t="s">
+        <v>6</v>
+      </c>
       <c r="D65">
         <v>0.5</v>
       </c>
@@ -1857,10 +2106,13 @@
       </c>
       <c r="K65" s="1"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>79</v>
       </c>
+      <c r="B66" t="s">
+        <v>6</v>
+      </c>
       <c r="D66">
         <v>0.5</v>
       </c>
@@ -1869,10 +2121,13 @@
       </c>
       <c r="K66" s="1"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>80</v>
       </c>
+      <c r="B67" t="s">
+        <v>6</v>
+      </c>
       <c r="D67">
         <v>0.5</v>
       </c>
@@ -1881,10 +2136,13 @@
       </c>
       <c r="K67" s="1"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>81</v>
       </c>
+      <c r="B68" t="s">
+        <v>6</v>
+      </c>
       <c r="D68">
         <v>0.5</v>
       </c>
@@ -1893,10 +2151,13 @@
       </c>
       <c r="K68" s="1"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>82</v>
       </c>
+      <c r="B69" t="s">
+        <v>6</v>
+      </c>
       <c r="D69">
         <v>0.5</v>
       </c>
@@ -1905,10 +2166,13 @@
       </c>
       <c r="K69" s="1"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>83</v>
       </c>
+      <c r="B70" t="s">
+        <v>6</v>
+      </c>
       <c r="D70">
         <v>0.5</v>
       </c>
@@ -1917,10 +2181,13 @@
       </c>
       <c r="K70" s="1"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>84</v>
       </c>
+      <c r="B71" t="s">
+        <v>6</v>
+      </c>
       <c r="D71">
         <v>0.5</v>
       </c>
@@ -1929,10 +2196,13 @@
       </c>
       <c r="K71" s="1"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>85</v>
       </c>
+      <c r="B72" t="s">
+        <v>6</v>
+      </c>
       <c r="D72">
         <v>0.5</v>
       </c>
@@ -1941,10 +2211,13 @@
       </c>
       <c r="K72" s="1"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>86</v>
       </c>
+      <c r="B73" t="s">
+        <v>6</v>
+      </c>
       <c r="D73">
         <v>0.5</v>
       </c>
@@ -1953,10 +2226,13 @@
       </c>
       <c r="K73" s="1"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>87</v>
       </c>
+      <c r="B74" t="s">
+        <v>6</v>
+      </c>
       <c r="D74">
         <v>0.5</v>
       </c>
@@ -1965,10 +2241,13 @@
       </c>
       <c r="K74" s="1"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>88</v>
       </c>
+      <c r="B75" t="s">
+        <v>6</v>
+      </c>
       <c r="D75">
         <v>0.5</v>
       </c>
@@ -1977,7 +2256,344 @@
       </c>
       <c r="K75" s="1"/>
     </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>89</v>
+      </c>
+      <c r="C76">
+        <v>35</v>
+      </c>
+      <c r="D76">
+        <v>0.6</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="K76" s="1"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>90</v>
+      </c>
+      <c r="C77">
+        <v>36</v>
+      </c>
+      <c r="D77">
+        <v>0.65</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="K77" s="1"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>91</v>
+      </c>
+      <c r="C78">
+        <v>37</v>
+      </c>
+      <c r="D78">
+        <v>0.95</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="K78" s="1"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>92</v>
+      </c>
+      <c r="C79">
+        <v>35</v>
+      </c>
+      <c r="D79">
+        <v>0.75</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I79" s="1">
+        <v>10</v>
+      </c>
+      <c r="K79" s="1"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>95</v>
+      </c>
+      <c r="C80">
+        <v>41</v>
+      </c>
+      <c r="D80">
+        <v>0.75</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G80" s="1">
+        <v>10</v>
+      </c>
+      <c r="K80" s="1"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>96</v>
+      </c>
+      <c r="C81">
+        <v>36</v>
+      </c>
+      <c r="D81">
+        <v>0.6</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H81" s="1">
+        <v>10</v>
+      </c>
+      <c r="K81" s="1"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>97</v>
+      </c>
+      <c r="C82">
+        <v>37</v>
+      </c>
+      <c r="D82">
+        <v>0.6</v>
+      </c>
+      <c r="G82" s="1">
+        <v>10</v>
+      </c>
+      <c r="K82" s="1"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>98</v>
+      </c>
+      <c r="C83">
+        <v>39</v>
+      </c>
+      <c r="D83">
+        <v>0.6</v>
+      </c>
+      <c r="G83" s="1">
+        <v>10</v>
+      </c>
+      <c r="K83" s="1"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>99</v>
+      </c>
+      <c r="C84">
+        <v>43</v>
+      </c>
+      <c r="D84">
+        <v>0.6</v>
+      </c>
+      <c r="K84" s="1"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>100</v>
+      </c>
+      <c r="C85">
+        <v>35</v>
+      </c>
+      <c r="D85">
+        <v>3</v>
+      </c>
+      <c r="H85" s="1">
+        <v>10</v>
+      </c>
+      <c r="K85" s="1"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>101</v>
+      </c>
+      <c r="C86">
+        <v>37</v>
+      </c>
+      <c r="D86">
+        <v>3</v>
+      </c>
+      <c r="G86" s="1">
+        <v>10</v>
+      </c>
+      <c r="K86" s="1"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>102</v>
+      </c>
+      <c r="C87">
+        <v>39</v>
+      </c>
+      <c r="D87">
+        <v>3</v>
+      </c>
+      <c r="G87" s="1">
+        <v>10</v>
+      </c>
+      <c r="K87" s="1"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>103</v>
+      </c>
+      <c r="C88">
+        <v>41</v>
+      </c>
+      <c r="D88">
+        <v>3</v>
+      </c>
+      <c r="G88" s="1">
+        <v>10</v>
+      </c>
+      <c r="K88" s="1"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>104</v>
+      </c>
+      <c r="C89">
+        <v>43</v>
+      </c>
+      <c r="D89">
+        <v>3</v>
+      </c>
+      <c r="G89" s="1">
+        <v>10</v>
+      </c>
+      <c r="K89" s="1"/>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>105</v>
+      </c>
+      <c r="C90">
+        <v>35</v>
+      </c>
+      <c r="D90">
+        <v>0.95</v>
+      </c>
+      <c r="G90" s="1">
+        <v>10</v>
+      </c>
+      <c r="K90" s="1"/>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>106</v>
+      </c>
+      <c r="C91">
+        <v>38</v>
+      </c>
+      <c r="D91">
+        <v>0.95</v>
+      </c>
+      <c r="G91" s="1">
+        <v>10</v>
+      </c>
+      <c r="K91" s="1"/>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>107</v>
+      </c>
+      <c r="C92">
+        <v>43</v>
+      </c>
+      <c r="D92">
+        <v>0.95</v>
+      </c>
+      <c r="G92" s="1">
+        <v>10</v>
+      </c>
+      <c r="K92" s="1"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>108</v>
+      </c>
+      <c r="C93">
+        <v>36</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
+      </c>
+      <c r="E93">
+        <v>10</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G93" s="1">
+        <v>10</v>
+      </c>
+      <c r="K93" s="1"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>109</v>
+      </c>
+      <c r="C94">
+        <v>36</v>
+      </c>
+      <c r="D94">
+        <v>1.2</v>
+      </c>
+      <c r="E94">
+        <v>10</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H94" s="1">
+        <v>2</v>
+      </c>
+      <c r="I94" s="1">
+        <v>2</v>
+      </c>
+      <c r="K94" s="1"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>110</v>
+      </c>
+      <c r="C95">
+        <v>36</v>
+      </c>
+      <c r="D95">
+        <v>1.2</v>
+      </c>
+      <c r="E95">
+        <v>2</v>
+      </c>
+      <c r="F95" s="1">
+        <v>10</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="K95" s="1"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Reset modbase for work on CHI
</commit_message>
<xml_diff>
--- a/BiceExpanded EXTRAS/BICE Tech List.xlsx
+++ b/BiceExpanded EXTRAS/BICE Tech List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chimera\Documents\Paradox Interactive\Hearts of Iron IV\mod\BlackICE-Expanded\BiceExpanded EXTRAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James Rankin\Documents\Paradox Interactive\Hearts of Iron IV\mod\BlackICE-Expanded\BiceExpanded EXTRAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3472DC-66E2-488C-8501-50EB389F863F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA6CC22-E76D-4BC1-93D5-510E5BF18143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22296" windowHeight="13176" xr2:uid="{120BDE58-771D-4E2C-9FD2-0BCD9B5D8EC1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28080" windowHeight="16440" xr2:uid="{120BDE58-771D-4E2C-9FD2-0BCD9B5D8EC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Industry" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="112">
   <si>
     <t>Tech Name</t>
   </si>
@@ -375,7 +375,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -385,6 +385,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -410,16 +417,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -449,7 +471,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{042549B0-C838-440F-910F-E3E035F893B0}" name="Table1" displayName="Table1" ref="A1:K95" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{042549B0-C838-440F-910F-E3E035F893B0}" name="Table1" displayName="Table1" ref="A1:K95" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:K95" xr:uid="{C89E43BA-120F-4DC0-A6DA-5AF10A372DE6}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{BBD0135A-950C-45DB-9EA8-B23A1432BFFE}" name="Tech Name"/>
@@ -457,12 +479,12 @@
     <tableColumn id="3" xr3:uid="{ED58554E-F065-4A71-9C70-D140F04B9A92}" name="Year"/>
     <tableColumn id="4" xr3:uid="{C42EDC2F-B10A-4E06-9BAD-D1BED39BF075}" name="Cost"/>
     <tableColumn id="5" xr3:uid="{EF34E1DB-526B-4321-8E8F-8ED6B1249A52}" name="Base Prio"/>
-    <tableColumn id="11" xr3:uid="{A9BE7041-1DA8-4CF6-AD2E-9F1AC88CB0BC}" name="Prio -Y" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{83836DF1-0FD8-42BF-95BF-5D3393BBA7C1}" name="Prio 0 Y" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{C68A9217-D82C-45F2-A251-97E2E2917B20}" name="Prio 1 Y" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{F4EF635C-ED33-432F-8C8E-6A5920099464}" name="Prio 2 Y" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{A9BE7041-1DA8-4CF6-AD2E-9F1AC88CB0BC}" name="Prio -Y" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{83836DF1-0FD8-42BF-95BF-5D3393BBA7C1}" name="Prio 0 Y" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{C68A9217-D82C-45F2-A251-97E2E2917B20}" name="Prio 1 Y" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{F4EF635C-ED33-432F-8C8E-6A5920099464}" name="Prio 2 Y" dataDxfId="2"/>
     <tableColumn id="6" xr3:uid="{316272FF-89BD-4226-A0EA-7EC288C6978B}" name="Total Prio"/>
-    <tableColumn id="10" xr3:uid="{432739BE-3B67-46D6-97BE-16B6F8A629E7}" name="% Change" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{432739BE-3B67-46D6-97BE-16B6F8A629E7}" name="% Change" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -767,59 +789,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C3C70DF-FE6D-4113-A583-B190C327E009}">
   <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" customWidth="1"/>
-    <col min="3" max="3" width="6.109375" customWidth="1"/>
-    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="1" customWidth="1"/>
-    <col min="7" max="9" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1"/>
-    <col min="11" max="11" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="1" customWidth="1"/>
+    <col min="7" max="9" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -837,7 +859,7 @@
       </c>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -858,7 +880,7 @@
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -885,7 +907,7 @@
       </c>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -909,7 +931,7 @@
       </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -930,7 +952,7 @@
       </c>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -957,7 +979,7 @@
       </c>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -978,7 +1000,7 @@
       </c>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -999,7 +1021,7 @@
       </c>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1020,7 +1042,7 @@
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1047,7 +1069,7 @@
       </c>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1068,7 +1090,7 @@
       </c>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1089,7 +1111,7 @@
       </c>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1110,7 +1132,7 @@
       </c>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1131,7 +1153,7 @@
       </c>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1149,7 +1171,7 @@
       </c>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1170,7 +1192,7 @@
       </c>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1194,7 +1216,7 @@
       </c>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -1218,7 +1240,7 @@
       </c>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1242,7 +1264,7 @@
       </c>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1266,7 +1288,7 @@
       </c>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1284,7 +1306,7 @@
       </c>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1308,7 +1330,7 @@
       </c>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -1329,7 +1351,7 @@
       </c>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -1353,7 +1375,7 @@
       </c>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1371,7 +1393,7 @@
       </c>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1389,7 +1411,7 @@
       </c>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -1413,7 +1435,7 @@
       </c>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -1437,7 +1459,7 @@
       </c>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -1461,7 +1483,7 @@
       </c>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -1485,7 +1507,7 @@
       </c>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1506,7 +1528,7 @@
       </c>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -1530,7 +1552,7 @@
       </c>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -1554,7 +1576,7 @@
       </c>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>47</v>
       </c>
@@ -1578,7 +1600,7 @@
       </c>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>49</v>
       </c>
@@ -1602,7 +1624,7 @@
       </c>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>50</v>
       </c>
@@ -1626,7 +1648,7 @@
       </c>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>51</v>
       </c>
@@ -1650,7 +1672,7 @@
       </c>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -1674,7 +1696,7 @@
       </c>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>53</v>
       </c>
@@ -1698,7 +1720,7 @@
       </c>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -1722,7 +1744,7 @@
       </c>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>55</v>
       </c>
@@ -1746,7 +1768,7 @@
       </c>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>56</v>
       </c>
@@ -1764,7 +1786,7 @@
       </c>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>57</v>
       </c>
@@ -1785,7 +1807,7 @@
       </c>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -1806,7 +1828,7 @@
       </c>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>59</v>
       </c>
@@ -1821,7 +1843,7 @@
       </c>
       <c r="K46" s="1"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>60</v>
       </c>
@@ -1836,7 +1858,7 @@
       </c>
       <c r="K47" s="1"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>61</v>
       </c>
@@ -1851,7 +1873,7 @@
       </c>
       <c r="K48" s="1"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>62</v>
       </c>
@@ -1866,7 +1888,7 @@
       </c>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -1881,7 +1903,7 @@
       </c>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>64</v>
       </c>
@@ -1896,7 +1918,7 @@
       </c>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>65</v>
       </c>
@@ -1911,7 +1933,7 @@
       </c>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>66</v>
       </c>
@@ -1926,7 +1948,7 @@
       </c>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>67</v>
       </c>
@@ -1941,7 +1963,7 @@
       </c>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>68</v>
       </c>
@@ -1956,7 +1978,7 @@
       </c>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>69</v>
       </c>
@@ -1971,7 +1993,7 @@
       </c>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -1986,7 +2008,7 @@
       </c>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>71</v>
       </c>
@@ -2001,7 +2023,7 @@
       </c>
       <c r="K58" s="1"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>72</v>
       </c>
@@ -2016,7 +2038,7 @@
       </c>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>73</v>
       </c>
@@ -2031,7 +2053,7 @@
       </c>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>74</v>
       </c>
@@ -2046,7 +2068,7 @@
       </c>
       <c r="K61" s="1"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>75</v>
       </c>
@@ -2061,7 +2083,7 @@
       </c>
       <c r="K62" s="1"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>76</v>
       </c>
@@ -2076,7 +2098,7 @@
       </c>
       <c r="K63" s="1"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>77</v>
       </c>
@@ -2091,7 +2113,7 @@
       </c>
       <c r="K64" s="1"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>78</v>
       </c>
@@ -2106,7 +2128,7 @@
       </c>
       <c r="K65" s="1"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>79</v>
       </c>
@@ -2121,7 +2143,7 @@
       </c>
       <c r="K66" s="1"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>80</v>
       </c>
@@ -2136,7 +2158,7 @@
       </c>
       <c r="K67" s="1"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>81</v>
       </c>
@@ -2151,7 +2173,7 @@
       </c>
       <c r="K68" s="1"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>82</v>
       </c>
@@ -2166,7 +2188,7 @@
       </c>
       <c r="K69" s="1"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>83</v>
       </c>
@@ -2181,7 +2203,7 @@
       </c>
       <c r="K70" s="1"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>84</v>
       </c>
@@ -2196,7 +2218,7 @@
       </c>
       <c r="K71" s="1"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>85</v>
       </c>
@@ -2211,7 +2233,7 @@
       </c>
       <c r="K72" s="1"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>86</v>
       </c>
@@ -2226,7 +2248,7 @@
       </c>
       <c r="K73" s="1"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>87</v>
       </c>
@@ -2241,7 +2263,7 @@
       </c>
       <c r="K74" s="1"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>88</v>
       </c>
@@ -2256,10 +2278,13 @@
       </c>
       <c r="K75" s="1"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>89</v>
       </c>
+      <c r="B76" t="s">
+        <v>6</v>
+      </c>
       <c r="C76">
         <v>35</v>
       </c>
@@ -2271,10 +2296,13 @@
       </c>
       <c r="K76" s="1"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>90</v>
       </c>
+      <c r="B77" t="s">
+        <v>6</v>
+      </c>
       <c r="C77">
         <v>36</v>
       </c>
@@ -2286,10 +2314,13 @@
       </c>
       <c r="K77" s="1"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>91</v>
       </c>
+      <c r="B78" t="s">
+        <v>6</v>
+      </c>
       <c r="C78">
         <v>37</v>
       </c>
@@ -2301,10 +2332,13 @@
       </c>
       <c r="K78" s="1"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>92</v>
       </c>
+      <c r="B79" t="s">
+        <v>6</v>
+      </c>
       <c r="C79">
         <v>35</v>
       </c>
@@ -2322,10 +2356,13 @@
       </c>
       <c r="K79" s="1"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>95</v>
       </c>
+      <c r="B80" t="s">
+        <v>6</v>
+      </c>
       <c r="C80">
         <v>41</v>
       </c>
@@ -2343,10 +2380,13 @@
       </c>
       <c r="K80" s="1"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>96</v>
       </c>
+      <c r="B81" t="s">
+        <v>6</v>
+      </c>
       <c r="C81">
         <v>36</v>
       </c>
@@ -2364,10 +2404,13 @@
       </c>
       <c r="K81" s="1"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>97</v>
       </c>
+      <c r="B82" t="s">
+        <v>6</v>
+      </c>
       <c r="C82">
         <v>37</v>
       </c>
@@ -2379,10 +2422,13 @@
       </c>
       <c r="K82" s="1"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>98</v>
       </c>
+      <c r="B83" t="s">
+        <v>6</v>
+      </c>
       <c r="C83">
         <v>39</v>
       </c>
@@ -2394,10 +2440,13 @@
       </c>
       <c r="K83" s="1"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>99</v>
       </c>
+      <c r="B84" t="s">
+        <v>6</v>
+      </c>
       <c r="C84">
         <v>43</v>
       </c>
@@ -2406,10 +2455,13 @@
       </c>
       <c r="K84" s="1"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>100</v>
       </c>
+      <c r="B85" t="s">
+        <v>6</v>
+      </c>
       <c r="C85">
         <v>35</v>
       </c>
@@ -2421,10 +2473,13 @@
       </c>
       <c r="K85" s="1"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>101</v>
       </c>
+      <c r="B86" t="s">
+        <v>6</v>
+      </c>
       <c r="C86">
         <v>37</v>
       </c>
@@ -2436,10 +2491,13 @@
       </c>
       <c r="K86" s="1"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>102</v>
       </c>
+      <c r="B87" t="s">
+        <v>6</v>
+      </c>
       <c r="C87">
         <v>39</v>
       </c>
@@ -2451,10 +2509,13 @@
       </c>
       <c r="K87" s="1"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>103</v>
       </c>
+      <c r="B88" t="s">
+        <v>6</v>
+      </c>
       <c r="C88">
         <v>41</v>
       </c>
@@ -2466,10 +2527,13 @@
       </c>
       <c r="K88" s="1"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>104</v>
       </c>
+      <c r="B89" t="s">
+        <v>6</v>
+      </c>
       <c r="C89">
         <v>43</v>
       </c>
@@ -2481,10 +2545,13 @@
       </c>
       <c r="K89" s="1"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>105</v>
       </c>
+      <c r="B90" t="s">
+        <v>6</v>
+      </c>
       <c r="C90">
         <v>35</v>
       </c>
@@ -2496,10 +2563,13 @@
       </c>
       <c r="K90" s="1"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>106</v>
       </c>
+      <c r="B91" t="s">
+        <v>6</v>
+      </c>
       <c r="C91">
         <v>38</v>
       </c>
@@ -2511,10 +2581,13 @@
       </c>
       <c r="K91" s="1"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>107</v>
       </c>
+      <c r="B92" t="s">
+        <v>6</v>
+      </c>
       <c r="C92">
         <v>43</v>
       </c>
@@ -2526,10 +2599,13 @@
       </c>
       <c r="K92" s="1"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>108</v>
       </c>
+      <c r="B93" t="s">
+        <v>6</v>
+      </c>
       <c r="C93">
         <v>36</v>
       </c>
@@ -2547,10 +2623,13 @@
       </c>
       <c r="K93" s="1"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>109</v>
       </c>
+      <c r="B94" t="s">
+        <v>6</v>
+      </c>
       <c r="C94">
         <v>36</v>
       </c>
@@ -2571,9 +2650,12 @@
       </c>
       <c r="K94" s="1"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>110</v>
+      </c>
+      <c r="B95" t="s">
+        <v>6</v>
       </c>
       <c r="C95">
         <v>36</v>

</xml_diff>